<commit_message>
Token/Exit System Settings Changes
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\weighbridge-v1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBA900E-4380-45B9-95CC-66A82CFD94C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38603033-C2D6-41E9-9D06-9B1D0D1A39B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="732" windowWidth="30720" windowHeight="16548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weighing - Full Report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Sl.No</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Phone No</t>
+  </si>
+  <si>
+    <t>Round off</t>
+  </si>
+  <si>
+    <t>Credit</t>
   </si>
 </sst>
 </file>
@@ -84,9 +96,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm\ AM/PM"/>
-    <numFmt numFmtId="169" formatCode="dd\-mm\-yyyy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy\ hh:mm\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -122,9 +134,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,36 +451,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.53125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.59765625" customWidth="1"/>
-    <col min="14" max="14" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.53125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,46 +504,58 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -535,26 +563,11 @@
       <c r="C2" s="2">
         <v>44275</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
         <v>44274.527083333334</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>44274.027083333334</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -562,14 +575,14 @@
       <c r="P2" s="4">
         <v>44274.027083333334</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <v>44274.027083333334</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-2</v>
       </c>
@@ -577,26 +590,11 @@
       <c r="C3" s="2">
         <v>44275</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
         <v>44274.527083333334</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>44274.027083333334</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -604,14 +602,14 @@
       <c r="P3" s="4">
         <v>44274.027083333334</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4">
+        <v>44274.027083333334</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-3</v>
       </c>
@@ -619,26 +617,11 @@
       <c r="C4" s="2">
         <v>44275</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
         <v>44274.527083333334</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>44274.027083333334</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -646,11 +629,11 @@
       <c r="P4" s="4">
         <v>44274.027083333334</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <v>44274.027083333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>